<commit_message>
character select button fixes
</commit_message>
<xml_diff>
--- a/perkinites.xlsx
+++ b/perkinites.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="159">
   <si>
     <t>NC</t>
   </si>
@@ -472,6 +472,27 @@
   </si>
   <si>
     <t>Shielded single-target fighter</t>
+  </si>
+  <si>
+    <t>Chris Piette</t>
+  </si>
+  <si>
+    <t>David Romero</t>
+  </si>
+  <si>
+    <t>Side Burn</t>
+  </si>
+  <si>
+    <t>Lift Lid</t>
+  </si>
+  <si>
+    <t>Troll</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>DR</t>
   </si>
 </sst>
 </file>
@@ -814,11 +835,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X127"/>
+  <dimension ref="A1:X135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1579,98 +1600,79 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="1" t="s">
-        <v>18</v>
+        <v>152</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="A46" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>153</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+        <v>158</v>
+      </c>
     </row>
     <row r="51" spans="1:24">
       <c r="A51" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
     </row>
     <row r="55" spans="1:24">
       <c r="A55" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="1"/>
-      <c r="W55" s="1"/>
-      <c r="X55" s="1"/>
     </row>
     <row r="59" spans="1:24">
       <c r="A59" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -1685,11 +1687,9 @@
     </row>
     <row r="63" spans="1:24">
       <c r="A63" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -1709,23 +1709,20 @@
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
     </row>
     <row r="67" spans="1:22">
       <c r="A67" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -1740,14 +1737,12 @@
     </row>
     <row r="71" spans="1:22">
       <c r="A71" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>48</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -1765,18 +1760,19 @@
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
     </row>
     <row r="75" spans="1:22">
       <c r="A75" s="1" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D75" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -1789,34 +1785,21 @@
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
     </row>
-    <row r="76" spans="1:22">
-      <c r="A76" t="s">
-        <v>62</v>
-      </c>
-      <c r="N76" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22">
-      <c r="A77" t="s">
-        <v>63</v>
-      </c>
-      <c r="N77" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="79" spans="1:22">
       <c r="A79" s="1" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C79" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -1830,19 +1813,26 @@
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
       <c r="P79" s="1"/>
+      <c r="Q79" s="1"/>
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
-      <c r="V79" s="1"/>
     </row>
     <row r="83" spans="1:23">
       <c r="A83" s="1" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C83" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -1854,31 +1844,29 @@
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
-      <c r="V83" s="1"/>
-      <c r="W83" s="1"/>
     </row>
     <row r="84" spans="1:23">
       <c r="A84" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="N84" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:23">
       <c r="A85" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="N85" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87" spans="1:23">
       <c r="A87" s="1" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -1901,47 +1889,104 @@
     </row>
     <row r="91" spans="1:23">
       <c r="A91" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="S91" s="1"/>
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+    </row>
+    <row r="92" spans="1:23">
+      <c r="A92" t="s">
+        <v>36</v>
+      </c>
+      <c r="N92" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23">
+      <c r="A93" t="s">
+        <v>37</v>
+      </c>
+      <c r="N93" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="95" spans="1:23">
       <c r="A95" s="1" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
-    </row>
-    <row r="99" spans="1:22" s="1" customFormat="1"/>
-    <row r="103" spans="1:22" s="1" customFormat="1"/>
-    <row r="104" spans="1:22">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-    </row>
-    <row r="107" spans="1:22">
-      <c r="U107" s="1"/>
-      <c r="V107" s="1"/>
-    </row>
-    <row r="111" spans="1:22">
-      <c r="U111" s="1"/>
-      <c r="V111" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
+      <c r="G103" s="1"/>
+    </row>
+    <row r="107" spans="1:7" s="1" customFormat="1"/>
+    <row r="111" spans="1:7" s="1" customFormat="1"/>
+    <row r="112" spans="1:7">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
     </row>
     <row r="115" spans="21:22">
       <c r="U115" s="1"/>
+      <c r="V115" s="1"/>
     </row>
     <row r="119" spans="21:22">
       <c r="U119" s="1"/>
@@ -1949,11 +1994,18 @@
     </row>
     <row r="123" spans="21:22">
       <c r="U123" s="1"/>
-      <c r="V123" s="1"/>
     </row>
     <row r="127" spans="21:22">
       <c r="U127" s="1"/>
       <c r="V127" s="1"/>
+    </row>
+    <row r="131" spans="21:22">
+      <c r="U131" s="1"/>
+      <c r="V131" s="1"/>
+    </row>
+    <row r="135" spans="21:22">
+      <c r="U135" s="1"/>
+      <c r="V135" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>